<commit_message>
Add Dmg Red B to buffs
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5.119489145234795</t>
+          <t>9.761091559169799</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>LR_PHY_Buu_Bois</t>
+          <t>DFLR_PHY_Buu_Bois</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>16.88881714613055</t>
+          <t>20.550341814468673</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>LR_STR_GT_Duo</t>
+          <t>DFLR_STR_GT_Duo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4.602065457321771</t>
+          <t>5.100269432844584</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LR_TEQ_Fusion_Zamasu</t>
+          <t>DFLR_TEQ_Fusion_Zamasu</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>94.64603469490743</t>
+          <t>89.05775365126465</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>23.1966119657344</t>
+          <t>28.360934907238175</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>12.831383098427764</t>
+          <t>12.367395542094705</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14.164681246660392</t>
+          <t>15.54309710321133</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>82.57898631023029</t>
+          <t>64.33532095603707</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4.161636520099421</t>
+          <t>7.773118256406022</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,161 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3.3196996008513815</t>
+          <t>6.303014270008721</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DF_INT_ToP_Androids</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>28.0987740482617</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BU_STR_Universe_2</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DF_AGL_Berserk_Kale</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>7.571905174214976</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>DF_PHY_God_Goku</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>14.912581234610627</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DF_PHY_Kid_Goku</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>29.12503072830121</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DF_TEQ_Fusing_Kefla</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>20.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>DF_STR_Costume_Videl</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>5.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Goku Black Banner
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\DokkanAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AE3626-950A-44B7-A84D-8365EECFB3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A6A715-7E9F-4561-8888-D1AFD2C41742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -437,6 +437,150 @@
   </si>
   <si>
     <t>CLR_PHY_Gogeta_Blue</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>BU_PHY_Gohan_Teen</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>BU_PHY_Super_Buu</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>BU_AGL_Pan_GT</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>BU_AGL_General_Rilldo</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>BU_STR_SS_Cabba</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>BU_STR_Hit_</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>BU_TEQ_Tien_</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>BU_TEQ_2ndForm_Cell</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>BU_INT_Kid_Gohan</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>BU_INT_Namek_Vegeta</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>LR_TEQ_SS3_Goku</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>CLR_INT_SS_Trio</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>LR_PHY_Android_Trio</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>DFLR_STR_Beast_Gohan</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>BU_AGL_Krillin_Android18</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>CLR_INT_Gammas_</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>DF_PHY_Goku_Black</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>DFLR_INT_Vegeta_Trunks</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>DF_INT_Future_Gohan</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>BU_STR_Future_Mai</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>BU_PHY_Gowasu_Zamasu</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>BU_PHY_Zamasu_</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>DFLR_AGL_MUI_Goku</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>DFLR_INT_EvoBlue_Vegeta</t>
   </si>
 </sst>
 </file>
@@ -621,16 +765,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DEBCCCA-EAC1-419C-8DD0-3BBC81E4B863}" name="Table1" displayName="Table1" ref="A1:D68" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="A1:D68" xr:uid="{4DEBCCCA-EAC1-419C-8DD0-3BBC81E4B863}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D68">
-    <sortCondition descending="1" ref="D1:D68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0FEF9C7E-91E2-44A9-92F4-EBBBFB648A27}" name="Table1" displayName="Table1" ref="A1:D92" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:D92" xr:uid="{0FEF9C7E-91E2-44A9-92F4-EBBBFB648A27}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D92">
+    <sortCondition descending="1" ref="D1:D92"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1C0F2F64-856D-4A6C-8BDC-A24E1DBAE3F3}" name="ID" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{4C513DDC-FF2B-4CA5-8D4D-2A0E5CEF73F6}" name="Common Name"/>
-    <tableColumn id="3" xr3:uid="{429A3662-531A-406D-8A15-EA015D1B036A}" name="# Copies"/>
-    <tableColumn id="4" xr3:uid="{084306BA-0C1D-4CFA-9D39-B9E42B1DF7A8}" name="Summon Rating"/>
+    <tableColumn id="1" xr3:uid="{24A5448C-BE72-4C01-9B68-5FA765127099}" name="ID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{B64D5E85-36D6-485D-AC15-B49C1333B6F7}" name="Common Name"/>
+    <tableColumn id="3" xr3:uid="{9C94F3AE-624C-414D-A1B2-98EF1F1DFE54}" name="# Copies"/>
+    <tableColumn id="4" xr3:uid="{A9F172DA-28EF-4041-83AE-3A3B14407870}" name="Summon Rating"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -921,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -950,44 +1094,44 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2">
-        <v>97.289028294785098</v>
+        <v>98.022791969058602</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3">
-        <v>87.111588280457596</v>
+        <v>96.495374875435004</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4">
-        <v>66.7162302824254</v>
+        <v>85.055648767041205</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -1001,119 +1145,119 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>66.173367480768405</v>
+        <v>62.287452463178298</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6">
-        <v>58.404595678348798</v>
+        <v>58.971861162038699</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7">
-        <v>37.314536194994602</v>
+        <v>55.3008264725526</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8">
-        <v>35.572172698369798</v>
+        <v>55.183099313816598</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9">
-        <v>25.474533440763899</v>
+        <v>42.797618346763898</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10">
-        <v>21.650107050428801</v>
+        <v>29.062581578640501</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11">
-        <v>21.131272104885198</v>
+        <v>27.691554700876399</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D12">
-        <v>20.850034715305899</v>
+        <v>23.600607159267501</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D13">
-        <v>18.601354765816101</v>
+        <v>23.511003663161901</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -1127,762 +1271,1098 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>18.2679421600415</v>
+        <v>20.174910457734601</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>17.999833336750701</v>
+        <v>19.240499008663299</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D16">
-        <v>13.868222670004601</v>
+        <v>16.844476417734501</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D17">
-        <v>13.588417901608301</v>
+        <v>16.349158732050501</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18">
-        <v>13.1893802705131</v>
+        <v>16.262813926256602</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19">
-        <v>12.8859814594589</v>
+        <v>14.204405241348001</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20">
-        <v>12.733009048835299</v>
+        <v>13.750329784951701</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>12.269960172870899</v>
+        <v>13.579073838291899</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>11.8369627941298</v>
+        <v>13.365643779770799</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23">
-        <v>11.6666666666666</v>
+        <v>13.3119237019917</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24">
-        <v>11.1609041340877</v>
+        <v>13.233046680733599</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25">
-        <v>10.0540333718135</v>
+        <v>12.971046056864401</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>155</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D26">
-        <v>9.9169089561652299</v>
+        <v>12.785916836244599</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27">
-        <v>9.1778231659976495</v>
+        <v>12.6178566953346</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D28">
-        <v>8.7721361902766404</v>
+        <v>11.8298659921367</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D29">
-        <v>8.0693539279991597</v>
+        <v>11.6666666666666</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>131</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30">
-        <v>7.80020529402496</v>
+        <v>11.5670437365851</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31">
-        <v>7.7558330044186903</v>
+        <v>11.408016765277599</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32">
-        <v>7.48717829743872</v>
+        <v>10.869052458020599</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33">
-        <v>6.7195086483953901</v>
+        <v>9.6066074326758901</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>6.5919615687956403</v>
+        <v>9.3761759717375295</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D35">
-        <v>6.2709605473800503</v>
+        <v>8.2997609121394902</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>163</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D36">
-        <v>6.14367825330587</v>
+        <v>7.85247831518359</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D37">
-        <v>6.08271645739402</v>
+        <v>7.3199674435065001</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D38">
-        <v>5.8691380601277601</v>
+        <v>6.9521253620835601</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39">
-        <v>5.6332727773910101</v>
+        <v>6.6998545492117598</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40">
-        <v>5.60064792754397</v>
+        <v>6.5226240495562697</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D41">
-        <v>5.51652602120976</v>
+        <v>6.3477442214732998</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>5.0267067982988296</v>
+        <v>5.7911200096659501</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43">
-        <v>4.3435066172070398</v>
+        <v>5.4597627790951702</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
       </c>
       <c r="D44">
-        <v>3.88888888888888</v>
+        <v>5.4519385305758199</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D45">
-        <v>3.4802198346159301</v>
+        <v>5.05429540757802</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46">
-        <v>3.1833180885313501</v>
+        <v>5.0410396600824701</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>31</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D47">
-        <v>3.1551464656112098</v>
+        <v>4.9976255404624901</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D48">
-        <v>3.1105053178457802</v>
+        <v>4.6486413553941697</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>176</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D49">
-        <v>2.5141742618609602</v>
+        <v>4.6221957927295003</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D50">
-        <v>2.5</v>
+        <v>4.4021357567781303</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D51">
-        <v>2.33659526928952</v>
+        <v>4.4019043011400703</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D52">
-        <v>2.3340224522152702</v>
+        <v>4.3603645422644801</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="C53" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D53">
-        <v>1.8789236961097799</v>
+        <v>4.1836348485379302</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="C54" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D54">
-        <v>1.6666666666666601</v>
+        <v>3.88888888888888</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="C55" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D55">
-        <v>1.6666666666666601</v>
+        <v>3.8157703791333</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D56">
-        <v>0.64814814814814703</v>
+        <v>3.4648028576480998</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>57</v>
+        <v>157</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="C57" t="s">
         <v>12</v>
       </c>
       <c r="D57">
-        <v>0.64814814814814703</v>
+        <v>3.4362522990822399</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="C58" t="s">
         <v>4</v>
       </c>
       <c r="D58">
-        <v>0.55555555555555503</v>
+        <v>3.3848706695484698</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D59">
-        <v>0.27777777777777701</v>
+        <v>3.2983788050727698</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C60" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D60">
-        <v>0.24605078861170401</v>
+        <v>3.2956759038100101</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D61">
-        <v>0.2</v>
+        <v>3.1371966377698</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C62" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D62">
-        <v>0.2</v>
+        <v>2.91498962976025</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D63">
-        <v>0.2</v>
+        <v>2.8557738182725201</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64">
-        <v>0.2</v>
+        <v>2.77896129611488</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="C65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D65">
-        <v>0.2</v>
+        <v>2.75496618181108</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>115</v>
+        <v>179</v>
       </c>
       <c r="B66" t="s">
-        <v>116</v>
+        <v>180</v>
       </c>
       <c r="C66" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D66">
-        <v>0.2</v>
+        <v>2.4655432270393001</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D67">
-        <v>0.2</v>
+        <v>2.4544420742647302</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68" t="s">
+        <v>102</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68">
+        <v>2.3881794717804898</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B69" t="s">
+        <v>160</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>2.1077973015887501</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B70" t="s">
+        <v>168</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70">
+        <v>2.0981509746717699</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A71" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" t="s">
+        <v>178</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71">
+        <v>1.6948660689989099</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A72" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" t="s">
+        <v>152</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72">
+        <v>1.6704665412926301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A73" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73">
+        <v>1.6666666666666601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74">
+        <v>1.6666666666666601</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B75" t="s">
+        <v>108</v>
+      </c>
+      <c r="C75" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75">
+        <v>1.5606830856595799</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A76" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76">
+        <v>1.27619381381577</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A77" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B77" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77">
+        <v>0.78170609828939897</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78">
+        <v>0.64814814814814703</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79">
+        <v>0.64814814814814703</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <v>0.55555555555555503</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A81" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B81" t="s">
+        <v>72</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81">
+        <v>0.27777777777777701</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A82" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" t="s">
+        <v>26</v>
+      </c>
+      <c r="C82" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A83" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A84" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" t="s">
+        <v>70</v>
+      </c>
+      <c r="C84" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A85" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>84</v>
+      </c>
+      <c r="C85" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A86" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" t="s">
+        <v>98</v>
+      </c>
+      <c r="C86" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A87" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B87" t="s">
+        <v>112</v>
+      </c>
+      <c r="C87" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A88" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B88" t="s">
+        <v>116</v>
+      </c>
+      <c r="C88" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A89" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B89" t="s">
+        <v>122</v>
+      </c>
+      <c r="C89" t="s">
+        <v>13</v>
+      </c>
+      <c r="D89">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A90" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B90" t="s">
         <v>124</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C90" t="s">
         <v>13</v>
       </c>
-      <c r="D68">
+      <c r="D90">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A91" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A92" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B92" t="s">
+        <v>186</v>
+      </c>
+      <c r="C92" t="s">
+        <v>13</v>
+      </c>
+      <c r="D92">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimise and summoning update
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>13.972514902832145</t>
+          <t>14.133340412625804</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>19.410838986358154</t>
+          <t>19.077895625846853</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>16.650310174391976</t>
+          <t>16.868613330468833</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11.539487960232243</t>
+          <t>10.352530283634735</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10.92740889203912</t>
+          <t>10.34971053072163</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6.691451999173708</t>
+          <t>6.510814244639059</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5.711740702908826</t>
+          <t>5.578333906768179</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>7.219838303694438</t>
+          <t>7.309310127153189</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.988977739627039</t>
+          <t>10.940510380601005</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.8384657405812717</t>
+          <t>2.6268567181014317</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22.72467347850123</t>
+          <t>22.2859941312868</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>9.45539082548779</t>
+          <t>9.389287054125319</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14.198148175704631</t>
+          <t>14.190860551586304</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>11.3636599358607</t>
+          <t>10.98307009639102</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4.609374730635527</t>
+          <t>4.082528974969949</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>27.93713354888283</t>
+          <t>27.08002772244592</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>22.73258870469467</t>
+          <t>21.97372854706214</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4.48789194612867</t>
+          <t>4.462902158067706</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>7.5120981025986335</t>
+          <t>7.114561657913072</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>16.2595112082838</t>
+          <t>15.724323622620199</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>9.155712695763006</t>
+          <t>8.877955651729955</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.982700694071748</t>
+          <t>2.685810565637707</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3.2700325082870787</t>
+          <t>3.067226924536795</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7.159001145377904</t>
+          <t>6.59582218088197</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>61.11789243840044</t>
+          <t>64.78687639641227</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14.021177050309134</t>
+          <t>14.134038143912903</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>13.697531098961761</t>
+          <t>13.745754425097564</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2.9026921747339287</t>
+          <t>2.83537508308558</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2.6152746899239623</t>
+          <t>2.5284272519392257</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>62.70960043427856</t>
+          <t>62.34850144228113</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>6.783749618205675</t>
+          <t>6.795075598727976</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12.05835809736988</t>
+          <t>11.34255459010593</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.1865071665576927</t>
+          <t>1.0477672544943877</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3.513698487640049</t>
+          <t>3.2532313569149847</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3.2186149367987724</t>
+          <t>3.2795068569092893</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2.106392065022155</t>
+          <t>2.1615896714057374</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6.797291489616786</t>
+          <t>6.865860983112577</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3.2202147483669443</t>
+          <t>2.921017307124261</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.427887581710476</t>
+          <t>1.2962962962962958</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>20.420389897583362</t>
+          <t>20.311560476932023</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>4.600513207820268</t>
+          <t>4.669913530351197</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>5.518224883595008</t>
+          <t>5.655445028056643</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5.058758282468045</t>
+          <t>4.900064301327429</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>4.30571430479678</t>
+          <t>4.117636032410978</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>3.6889718802432885</t>
+          <t>3.4799681180262105</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12.446786643714773</t>
+          <t>12.612343854748275</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>11.73672107134577</t>
+          <t>12.18306577064891</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>16.22300733610504</t>
+          <t>16.07008016401693</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>84.53678030551835</t>
+          <t>83.1312508532607</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>96.65576530942496</t>
+          <t>96.55930484816379</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2.525706534336909</t>
+          <t>2.3591775203152823</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4.080637633290956</t>
+          <t>3.831163045718534</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2.5473346699357378</t>
+          <t>2.383002484969857</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>3.8792378957230493</t>
+          <t>3.6776361212976343</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12.674919353436763</t>
+          <t>12.36190870176738</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>4.3319072378465915</t>
+          <t>4.128562334741663</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.5086634805707633</t>
+          <t>1.386542352415373</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>5.090311905066295</t>
+          <t>4.836681769311175</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>12.222203010965654</t>
+          <t>11.908048677191992</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>3.1851064819689223</t>
+          <t>2.974753956948206</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2.058174473298449</t>
+          <t>1.9379151650275726</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>41.87972829063806</t>
+          <t>39.31061310425023</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>8.304179304603709</t>
+          <t>8.179683151192107</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>98.01678357597685</t>
+          <t>98.09400349519292</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2.422463491454412</t>
+          <t>2.271869476881736</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>53.80327721004567</t>
+          <t>52.51537479829067</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>26.34169436548518</t>
+          <t>24.76966023485272</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>13.59317021085576</t>
+          <t>13.803210325440759</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>4.671748018887158</t>
+          <t>4.659542244013985</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.5467567232234287</t>
+          <t>1.4287527744381399</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.7500051326379014</t>
+          <t>2.7266508617553966</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>0.776438877854699</t>
+          <t>0.7004388124634752</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,205 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>11.857060478308021</t>
+          <t>11.798349300571095</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>DFLR_PHY_Buutenks_</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>95</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>DFLR_STR_SS_Vegito</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>BU_INT_Dodoria_</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>16.43953697967035</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>97</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DF_AGL_1stForm_Frieza</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>48.09467853489954</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>DF_AGL_SS_Bardock</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>BU_AGL_King_Vegeta</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>12.20756811006764</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>DF_TEQ_SS_Vegeta</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>75.73779918278534</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>101</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>DF_AGL_DragonFist_Goku</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>4.0054013442748255</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>DFLR_INT_SFPS4_Goku</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>5.968161313573148</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Teq SS vegeta active skill attack multiplier
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>14.133340412625804</t>
+          <t>14.132857333438793</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>19.077895625846853</t>
+          <t>19.078635313671487</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>16.868613330468833</t>
+          <t>16.86804957264372</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.352530283634735</t>
+          <t>10.352979166817128</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>10.34971053072163</t>
+          <t>10.35100322721796</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6.510814244639059</t>
+          <t>6.5104002628833495</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5.578333906768179</t>
+          <t>5.5784055063340965</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>7.309310127153189</t>
+          <t>7.308084443450454</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.940510380601005</t>
+          <t>10.941165841762583</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.6268567181014317</t>
+          <t>2.6268304323492213</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>22.2859941312868</t>
+          <t>22.2901640142887</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>9.389287054125319</t>
+          <t>9.389159900756226</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14.190860551586304</t>
+          <t>14.191060735235943</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10.98307009639102</t>
+          <t>10.985494960541278</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4.082528974969949</t>
+          <t>4.083060905109048</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>27.08002772244592</t>
+          <t>27.08307945869664</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>21.97372854706214</t>
+          <t>21.9791299340416</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4.462902158067706</t>
+          <t>4.462258580812701</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>7.114561657913072</t>
+          <t>7.1144524098602515</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15.724323622620199</t>
+          <t>15.72633295413688</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>8.877955651729955</t>
+          <t>8.876157870353966</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.685810565637707</t>
+          <t>2.686678092555963</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3.067226924536795</t>
+          <t>3.0680096503521805</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>6.59582218088197</t>
+          <t>6.596082923040191</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>64.78687639641227</t>
+          <t>64.78256506104303</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14.134038143912903</t>
+          <t>14.134553587646586</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>13.745754425097564</t>
+          <t>13.74467659989817</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2.83537508308558</t>
+          <t>2.8351612877348416</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2.5284272519392257</t>
+          <t>2.528322711879049</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>62.34850144228113</t>
+          <t>62.34615746532614</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>6.795075598727976</t>
+          <t>6.7937218939612976</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11.34255459010593</t>
+          <t>11.34285606471344</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.0477672544943877</t>
+          <t>1.0478559782110182</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3.2532313569149847</t>
+          <t>3.2537511408730624</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3.2795068569092893</t>
+          <t>28.037927745968446</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2.1615896714057374</t>
+          <t>2.1617461901411605</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6.865860983112577</t>
+          <t>6.865160109630305</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2.921017307124261</t>
+          <t>2.921401860711616</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>20.311560476932023</t>
+          <t>20.3115961545465</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>4.669913530351197</t>
+          <t>4.669968356634079</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>5.655445028056643</t>
+          <t>5.654864944514908</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4.900064301327429</t>
+          <t>4.900284055080419</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>4.117636032410978</t>
+          <t>4.117522396646869</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>3.4799681180262105</t>
+          <t>3.48046501322629</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>12.612343854748275</t>
+          <t>12.612790636182957</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12.18306577064891</t>
+          <t>12.181641524022865</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>16.07008016401693</t>
+          <t>16.06909372770657</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>83.1312508532607</t>
+          <t>83.13221356728918</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>96.55930484816379</t>
+          <t>96.55924705790383</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2.3591775203152823</t>
+          <t>2.359899243802385</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3.831163045718534</t>
+          <t>3.83224625823254</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2.383002484969857</t>
+          <t>2.383768508382552</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>3.6776361212976343</t>
+          <t>3.67853795375526</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>12.36190870176738</t>
+          <t>12.365358993764211</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>4.128562334741663</t>
+          <t>4.129497221360352</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.386542352415373</t>
+          <t>1.3869765361553135</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>4.836681769311175</t>
+          <t>4.8377838645686735</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>11.908048677191992</t>
+          <t>11.91122583150462</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2.974753956948206</t>
+          <t>2.9755835678819724</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.9379151650275726</t>
+          <t>11.791371934329248</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>39.31061310425023</t>
+          <t>39.32001335034202</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>8.179683151192107</t>
+          <t>8.179218536621091</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>98.09400349519292</t>
+          <t>98.09406650013413</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2.271869476881736</t>
+          <t>2.271762874101956</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>52.51537479829067</t>
+          <t>52.51438959676666</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>24.76966023485272</t>
+          <t>24.765808193381645</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>13.803210325440759</t>
+          <t>13.802628746663991</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>4.659542244013985</t>
+          <t>4.659457557810683</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.4287527744381399</t>
+          <t>1.4288398482509048</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.7266508617553966</t>
+          <t>2.7263747212195844</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>0.7004388124634752</t>
+          <t>0.7005651266453613</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>11.798349300571095</t>
+          <t>11.798381623277185</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>16.43953697967035</t>
+          <t>16.43805485276187</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>48.09467853489954</t>
+          <t>48.10705139526472</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>12.20756811006764</t>
+          <t>12.20922342273179</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>75.73779918278534</t>
+          <t>75.73586210801837</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>4.0054013442748255</t>
+          <t>4.005429435016678</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>5.968161313573148</t>
+          <t>6.24945950943237</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
1st Form Frieza Summons
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D163"/>
+  <dimension ref="A1:D188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11.831552161391901</t>
+          <t>11.663833691289161</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18.865243600830862</t>
+          <t>18.010432354973535</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17.045792397130548</t>
+          <t>17.837131774036884</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11.004678224411967</t>
+          <t>10.976376585653838</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>7.464498465816321</t>
+          <t>8.07692848685158</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>8.324405987640091</t>
+          <t>8.34944875296181</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3.244533343986805</t>
+          <t>3.1821858151560356</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>8.899597581246573</t>
+          <t>9.079257284880988</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>9.236140747099189</t>
+          <t>9.180197010715503</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.899051728084249</t>
+          <t>10.816402344229868</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.8457203378790603</t>
+          <t>1.9289052627888021</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12.37265568191357</t>
+          <t>12.30739668659515</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.27454729924090027</t>
+          <t>0.2951247212325932</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>10.870031590368622</t>
+          <t>10.74623823870914</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>15.944297737624375</t>
+          <t>15.632870201549451</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>8.904345282826338</t>
+          <t>8.510731179988824</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.6710216861779568</t>
+          <t>1.8334204926724222</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>5.269549312541744</t>
+          <t>5.309951431668836</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>19.26771015679671</t>
+          <t>19.36290716994727</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>19.23614383129296</t>
+          <t>19.8909654024957</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>7.5789712905802</t>
+          <t>7.414401812822788</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12.51544006339998</t>
+          <t>12.244879019549916</t>
         </is>
       </c>
     </row>
@@ -1062,12 +1062,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>16.86613355271769</t>
+          <t>11.765020173505818</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3.303007482302551</t>
+          <t>3.505336870477523</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.488697419459435</t>
+          <t>2.583253172261679</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3.946694174844686</t>
+          <t>3.9450266825332645</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>13.29380787023753</t>
+          <t>13.9459440069738</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7.277794574597735</t>
+          <t>7.044292563694667</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15.244862289977306</t>
+          <t>14.710758799952913</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4.278122515108052</t>
+          <t>4.233449871659474</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2.4643361213188903</t>
+          <t>2.44262478771531</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>9.636049484568034</t>
+          <t>9.373206922436196</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5.661725848335156</t>
+          <t>5.770579092523903</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.4334463134037372</t>
+          <t>1.474471322660532</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>6.892376094439616</t>
+          <t>7.008804635461907</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.349658915816568</t>
+          <t>1.328303261335029</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6.131079614005122</t>
+          <t>5.988475984576654</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2.5858726593845778</t>
+          <t>2.651753354301844</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.933836925594399</t>
+          <t>1.898101200847184</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>21.65213104079763</t>
+          <t>20.948399513955543</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3.3878580805698926</t>
+          <t>3.326578472533916</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4.87076700956093</t>
+          <t>2.452181224866032</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4.116088307066736</t>
+          <t>4.029809650341747</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3.7710823835607705</t>
+          <t>3.7375630933001105</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.8286921725011407</t>
+          <t>1.8664425952236348</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13.764561172489742</t>
+          <t>13.431866350304361</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12.198312601725787</t>
+          <t>12.069079893281241</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>9.167809410181473</t>
+          <t>9.596595944700887</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>66.665150477882</t>
+          <t>66.50062071847199</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>96.86286012267351</t>
+          <t>96.89033428563904</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2.339339401789047</t>
+          <t>2.514888377801021</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2.933814532843228</t>
+          <t>3.074200100867454</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2.1362095025487036</t>
+          <t>2.3648043934612706</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2.653835838749993</t>
+          <t>2.837814078396113</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>8.715771576707143</t>
+          <t>9.012856695338726</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3.0956932854922137</t>
+          <t>3.285813083414789</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.491315981658925</t>
+          <t>1.6377363222743135</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>3.6392120376778534</t>
+          <t>3.849099572933798</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>8.841385064732254</t>
+          <t>9.13884118324241</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2.9317733949160405</t>
+          <t>3.1643040302159555</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2.3875364035489377</t>
+          <t>2.2410436122285176</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>28.16101952371616</t>
+          <t>28.4133699292662</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>8.812451409825492</t>
+          <t>8.786672885306675</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>97.36032724035324</t>
+          <t>97.41493499755694</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>6.722314951447006</t>
+          <t>7.638149759067333</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>63.80449971194248</t>
+          <t>63.06786759934968</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>37.53481951924789</t>
+          <t>41.28549874711065</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>13.870203385418435</t>
+          <t>13.737462498371316</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>3.2418971919053305</t>
+          <t>3.27448237882845</t>
         </is>
       </c>
     </row>
@@ -2360,12 +2360,12 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.062932824070475</t>
+          <t>1.850962986830786</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>4.339769043271715</t>
+          <t>4.400940082399113</t>
         </is>
       </c>
     </row>
@@ -2404,12 +2404,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.557210736925179</t>
+          <t>2.296555417779827</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>10.235511923251384</t>
+          <t>10.39496434205949</t>
         </is>
       </c>
     </row>
@@ -2558,12 +2558,12 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>7.580369700791524</t>
+          <t>3.178620577306468</t>
         </is>
       </c>
     </row>
@@ -2580,12 +2580,12 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>33.96823159126019</t>
+          <t>19.252096036880747</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>8.0848461885901</t>
+          <t>8.53657746209501</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>58.90949790256493</t>
+          <t>58.96658321755441</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>8.439537914634345</t>
+          <t>9.868938065597492</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>9.084920892664798</t>
+          <t>9.168135381920365</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>3.145595345686149</t>
+          <t>3.1225862799667126</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>11.58740582811013</t>
+          <t>11.689874854284746</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>3.286035242495202</t>
+          <t>3.4731425721569</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>53.59419674411378</t>
+          <t>53.87866989328539</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2.182199159538662</t>
+          <t>2.161121166489931</t>
         </is>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>3.92061353850341</t>
+          <t>3.7693796075664614</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>1.7065828127292724</t>
+          <t>1.6484240849692453</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>3.120513788907431</t>
+          <t>3.0930739071694973</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>6.766507931208841</t>
+          <t>6.671750498526453</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>10.983909482628682</t>
+          <t>11.359121457155227</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>4.068130441077461</t>
+          <t>4.040086274706322</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>3.9293440943846907</t>
+          <t>4.115447265687816</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>0.7095955316784615</t>
+          <t>0.6907986685150674</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>7.34690326178181</t>
+          <t>7.6955453991733735</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2.243710352124539</t>
+          <t>2.1268983474332903</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2.770312790787763</t>
+          <t>2.883971357293909</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>1.7684220713826808</t>
+          <t>1.7372094676010446</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2.849292850082561</t>
+          <t>2.85942690877199</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>3.295011372180511</t>
+          <t>3.342395750932411</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2.0609874068856904</t>
+          <t>1.9796519230677987</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>7.902756037892871</t>
+          <t>7.628835899920812</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>4.329832805655142</t>
+          <t>4.253297159458121</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>6.806138018569181</t>
+          <t>6.431671567256396</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>10.534202809218332</t>
+          <t>10.598608910489745</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>6.268160989303597</t>
+          <t>4.304328904308898</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>5.655122541031831</t>
+          <t>5.60324181694959</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2.316418805196531</t>
+          <t>2.343980219410103</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>2.840730414097611</t>
+          <t>2.7634476419219314</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>4.406762494815183</t>
+          <t>4.344133515159922</t>
         </is>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>29.71939089954485</t>
+          <t>29.97006172294734</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>10.349995642106158</t>
+          <t>10.425668949150342</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>32.02084134397278</t>
+          <t>33.24785597148502</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>9.314485782358119</t>
+          <t>8.94990283094134</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>13.03949542959866</t>
+          <t>12.880942866287782</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,557 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>18.49955492714302</t>
+          <t>16.77437321608755</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="inlineStr">
+        <is>
+          <t>163</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>DF_TEQ_Exchange_Buu</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2.7299376954687853</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="inlineStr">
+        <is>
+          <t>164</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>DF_TEQ_Ultimate_Gohan</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="inlineStr">
+        <is>
+          <t>165</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>LR_AGL_Ultimate_Gohan</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>23.01141905249355</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="inlineStr">
+        <is>
+          <t>166</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>BU_INT_Hercule_</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="inlineStr">
+        <is>
+          <t>167</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>BU_PHY_Buutenks_</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="inlineStr">
+        <is>
+          <t>168</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>BU_INT_SS_Goten</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="inlineStr">
+        <is>
+          <t>169</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>BU_TEQ_Kid_Trunks</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>DF_PHY_Kid_Buu</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>9.865812410020636</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="inlineStr">
+        <is>
+          <t>171</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>DF_STR_SS3_Vegeta</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="inlineStr">
+        <is>
+          <t>172</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>BU_INT_Cheelai_</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>5.38438826496148</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="inlineStr">
+        <is>
+          <t>173</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>BU_PHY_Android_21</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2.9630865047527397</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="inlineStr">
+        <is>
+          <t>174</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>F2PLR_PHY_Babidi_Buu</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>F2P_PHY_Buyon_</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="inlineStr">
+        <is>
+          <t>176</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>F2P_PHY_Gohan_Goku</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="inlineStr">
+        <is>
+          <t>177</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>F2PLR_INT_Babidi_</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="inlineStr">
+        <is>
+          <t>178</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>BU_PHY_Robelu_</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="inlineStr">
+        <is>
+          <t>179</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>BU_PHY_Whirus_</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>F2P_PHY_UI_Goku</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>BU_PHY_Kid_Chichi</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>0.24228266550931224</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="inlineStr">
+        <is>
+          <t>182</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>BU_STR_Pan_GT</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="inlineStr">
+        <is>
+          <t>183</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>BU_STR_Whis_</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>BU_INT_Masked_King</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>4.325209282104981</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="inlineStr">
+        <is>
+          <t>185</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>BU_INT_Zamasu_</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>1.7624819467658195</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="inlineStr">
+        <is>
+          <t>186</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>BU_AGL_SS2_Trunks</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>6.296467248621603</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>F2PLR_TEQ_Trunks_Broly</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>0.2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Rework evaluation to use total damage instead of average per attack
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D188"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11.663833691289161</t>
+          <t>7.00125581793807</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18.010432354973535</t>
+          <t>18.18106152555067</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17.837131774036884</t>
+          <t>15.405470857358104</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.976376585653838</t>
+          <t>11.02527024434395</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>8.07692848685158</t>
+          <t>15.24629309802655</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.6481481481481479</t>
+          <t>1.223397094665883</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>8.34944875296181</t>
+          <t>4.56751784851377</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3.1821858151560356</t>
+          <t>3.0173208239170215</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>9.079257284880988</t>
+          <t>7.523022290725629</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>9.180197010715503</t>
+          <t>5.294391496089599</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>10.816402344229868</t>
+          <t>6.179548214014371</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.9289052627888021</t>
+          <t>2.328968768452001</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12.30739668659515</t>
+          <t>18.59358351616655</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.2951247212325932</t>
+          <t>0.647666530357951</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>10.74623823870914</t>
+          <t>6.960966425765491</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>15.632870201549451</t>
+          <t>13.867956926581197</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>8.510731179988824</t>
+          <t>9.963165664938009</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.8334204926724222</t>
+          <t>1.6666666666666665</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>5.309951431668836</t>
+          <t>10.50304467205885</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>19.36290716994727</t>
+          <t>13.31828235994885</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>19.8909654024957</t>
+          <t>23.69995088746306</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>7.414401812822788</t>
+          <t>5.746087006334193</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12.244879019549916</t>
+          <t>10.073704872497864</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.6481481481481479</t>
+          <t>1.161105319430709</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>11.765020173505818</t>
+          <t>8.66667164459012</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3.505336870477523</t>
+          <t>4.640470709578461</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.583253172261679</t>
+          <t>6.190018173070623</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3.9450266825332645</t>
+          <t>5.367560448078883</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>13.9459440069738</t>
+          <t>9.37542754743455</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.2777777777777778</t>
+          <t>0.3085772175724033</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7.044292563694667</t>
+          <t>10.368802560851293</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14.710758799952913</t>
+          <t>15.498391768041266</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4.233449871659474</t>
+          <t>4.305021780361216</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2.44262478771531</t>
+          <t>1.3153392264818216</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>9.373206922436196</t>
+          <t>9.229380821846753</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5.770579092523903</t>
+          <t>9.507924771580578</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.474471322660532</t>
+          <t>1.72490112816681</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>7.008804635461907</t>
+          <t>6.417439640237978</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.328303261335029</t>
+          <t>1.9576480770579963</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5.988475984576654</t>
+          <t>6.738294715590431</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2.651753354301844</t>
+          <t>3.669234327511709</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.898101200847184</t>
+          <t>5.179329421152897</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>20.948399513955543</t>
+          <t>16.90788902928376</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3.326578472533916</t>
+          <t>3.788260123247462</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2.452181224866032</t>
+          <t>2.68980340678425</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4.029809650341747</t>
+          <t>3.476848846862527</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3.7375630933001105</t>
+          <t>3.0246484155003017</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.8664425952236348</t>
+          <t>1.2504680436988096</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13.431866350304361</t>
+          <t>15.743417980337945</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>12.069079893281241</t>
+          <t>14.742251465731405</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>9.596595944700887</t>
+          <t>5.487777470589715</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>66.50062071847199</t>
+          <t>62.131923584303415</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>96.89033428563904</t>
+          <t>97.75432385995181</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2.514888377801021</t>
+          <t>5.281512175033996</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3.074200100867454</t>
+          <t>6.677186150993855</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2.3648043934612706</t>
+          <t>5.156567945015006</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2.837814078396113</t>
+          <t>6.3766929002507196</t>
         </is>
       </c>
     </row>
@@ -2030,12 +2030,12 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>9.012856695338726</t>
+          <t>10.949336838255695</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3.285813083414789</t>
+          <t>6.413516022363499</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.6377363222743135</t>
+          <t>4.2053747950115925</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>3.849099572933798</t>
+          <t>7.2934283404549065</t>
         </is>
       </c>
     </row>
@@ -2118,12 +2118,12 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>9.13884118324241</t>
+          <t>11.629762028953508</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>3.1643040302159555</t>
+          <t>6.275241514054455</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2.2410436122285176</t>
+          <t>2.2813165990281257</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>28.4133699292662</t>
+          <t>31.90215041013898</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>8.786672885306675</t>
+          <t>6.062142768927471</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>97.41493499755694</t>
+          <t>97.17369585216825</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>7.638149759067333</t>
+          <t>6.148021850146486</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>63.06786759934968</t>
+          <t>52.70714262584076</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>41.28549874711065</t>
+          <t>20.70708002724976</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>13.737462498371316</t>
+          <t>6.96550331865076</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>3.27448237882845</t>
+          <t>2.261882487645324</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.850962986830786</t>
+          <t>2.694072545987147</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>4.400940082399113</t>
+          <t>2.8015977724579972</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2.296555417779827</t>
+          <t>2.1535106112862357</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>10.39496434205949</t>
+          <t>9.720542863144471</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>3.178620577306468</t>
+          <t>2.3134371469143318</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>19.252096036880747</t>
+          <t>17.910813156441193</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>8.53657746209501</t>
+          <t>10.85451432016265</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>58.96658321755441</t>
+          <t>35.04874550692206</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>9.868938065597492</t>
+          <t>8.0926812297495</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>9.168135381920365</t>
+          <t>14.69523223640136</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>3.1225862799667126</t>
+          <t>3.718058546835266</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>3.8888888888888884</t>
+          <t>7.268226953783222</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>11.689874854284746</t>
+          <t>8.53875368311424</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>3.4731425721569</t>
+          <t>4.75178969675777</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>53.87866989328539</t>
+          <t>27.762573225063264</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2.161121166489931</t>
+          <t>1.2392089946503297</t>
         </is>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>3.7693796075664614</t>
+          <t>1.9458589733905547</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>1.6484240849692453</t>
+          <t>1.555481855357869</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>3.0930739071694973</t>
+          <t>2.5652075080612384</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>6.671750498526453</t>
+          <t>5.6276649566023655</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>11.359121457155227</t>
+          <t>7.316651835313637</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>4.040086274706322</t>
+          <t>2.5288039932725077</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>4.115447265687816</t>
+          <t>4.611418313649975</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>0.6907986685150674</t>
+          <t>0.7868324244146881</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>7.6955453991733735</t>
+          <t>5.064448938181682</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2.1268983474332903</t>
+          <t>1.0275081092310234</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2.883971357293909</t>
+          <t>1.7360583803464422</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>1.7372094676010446</t>
+          <t>2.186850504245083</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>2.85942690877199</t>
+          <t>1.6226885990956772</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>3.342395750932411</t>
+          <t>1.7646542352029062</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>1.9796519230677987</t>
+          <t>1.2431309730473306</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>7.628835899920812</t>
+          <t>5.189966230618012</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>4.253297159458121</t>
+          <t>3.357216905734619</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>6.431671567256396</t>
+          <t>4.637041361816966</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>10.598608910489745</t>
+          <t>7.296433888480809</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>4.304328904308898</t>
+          <t>5.743132279718387</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>5.60324181694959</t>
+          <t>3.8979447917578343</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2.343980219410103</t>
+          <t>1.4674930199345926</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>2.7634476419219314</t>
+          <t>2.5925324559983056</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>4.344133515159922</t>
+          <t>2.6187461360502176</t>
         </is>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>29.97006172294734</t>
+          <t>17.57663229286313</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>10.425668949150342</t>
+          <t>7.375423894911321</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>33.24785597148502</t>
+          <t>22.69168319193339</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>8.94990283094134</t>
+          <t>8.206030969521436</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>12.880942866287782</t>
+          <t>14.514306765888032</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>16.77437321608755</t>
+          <t>20.40767967911299</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>2.7299376954687853</t>
+          <t>2.8079386075396315</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>23.01141905249355</t>
+          <t>19.37982005758283</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>9.865812410020636</t>
+          <t>7.6734720005695545</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>5.38438826496148</t>
+          <t>3.774891872536209</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>2.9630865047527397</t>
+          <t>2.16905820169203</t>
         </is>
       </c>
     </row>
@@ -4433,7 +4433,7 @@
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>0.24228266550931224</t>
+          <t>0.21556458258495984</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>4.325209282104981</t>
+          <t>2.587934943265097</t>
         </is>
       </c>
     </row>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>1.7624819467658195</t>
+          <t>1.2131349573636137</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>6.296467248621603</t>
+          <t>6.560918731638093</t>
         </is>
       </c>
     </row>
@@ -4566,6 +4566,402 @@
       <c r="D188" t="inlineStr">
         <is>
           <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>BU_PHY_SS_Bardock</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>BU_PHY_WT_Tien</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>2.1887690444231502</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>BU_INT_Amond_Rasin</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>3.3304733042400247</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="inlineStr">
+        <is>
+          <t>191</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>F2P_INT_GT_Vegeta</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="inlineStr">
+        <is>
+          <t>192</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>BU_INT_Bota_Magetta</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>0.45120629558588554</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="inlineStr">
+        <is>
+          <t>193</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>DF_TEQ_Golden_Frieza</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>0.4323748579089417</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>BU_TEQ_Bulla_</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>BU_TEQ_Tapion_</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="inlineStr">
+        <is>
+          <t>196</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>F2P_TEQ_Candy_Vegito</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>F2P_TEQ_SS3_Goku</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="inlineStr">
+        <is>
+          <t>198</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>BU_INT_Whis_</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>0.8425460347912974</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="inlineStr">
+        <is>
+          <t>199</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>F2PLR_TEQ_Dragon_Ball</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>BU_INT_Future_Mai</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>F2P_INT_Bulma_Youth</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="inlineStr">
+        <is>
+          <t>202</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>BU_TEQ_Future_Gohan</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>BU_AGL_Daiz_Cacao</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>1.588571792364669</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="inlineStr">
+        <is>
+          <t>204</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>BU_AGL_GoldenMetal_Cooler</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>1.1252304447106596</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>BU_AGL_Baby_Janemba</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>4.919802248761799</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Temporary fix for Broly
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.383546099936529</t>
+          <t>6.37632562457711</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14.634324127024342</t>
+          <t>14.637989362345085</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15.79817369428104</t>
+          <t>15.810561449629022</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.292218606973776</t>
+          <t>10.269321654999558</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.431846660795866</t>
+          <t>2.427615066640635</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2.550616616523602</t>
+          <t>2.546548380998475</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.1981274565522995</t>
+          <t>4.2015699487283396</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.3471359001780394</t>
+          <t>2.34820770565918</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5.469687521711519</t>
+          <t>5.473564005455468</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6.424455860483661</t>
+          <t>6.430840546867309</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5.085396026800183</t>
+          <t>5.074897300499384</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.112077660399388</t>
+          <t>2.1098563988051193</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>12.7588908643051</t>
+          <t>12.68429271447673</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.770695734808178</t>
+          <t>0.7712496821925272</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6.8066508652153885</t>
+          <t>6.8115696071666</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10.855429779270368</t>
+          <t>10.851483964559458</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5.703745607959053</t>
+          <t>5.68214487220917</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1.7259517381505685</t>
+          <t>1.7281619174213612</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>7.053284035489621</t>
+          <t>7.050245004990942</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>8.541869171748704</t>
+          <t>8.530209824755405</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14.18193722237707</t>
+          <t>14.06608577073376</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>7.566513530381187</t>
+          <t>7.584452299997466</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6.341723403578616</t>
+          <t>6.349527232251154</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.985225413352753</t>
+          <t>1.982134295944779</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7.584287818150859</t>
+          <t>7.581071574418942</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4.383615487507941</t>
+          <t>4.386088009954863</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>5.359241516524241</t>
+          <t>5.342219454354002</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3.9544454070318107</t>
+          <t>3.9315233387901625</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>18.72040473915525</t>
+          <t>18.7355189998293</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12.716225390066489</t>
+          <t>12.72436054811363</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14.068107271475633</t>
+          <t>14.077351771980636</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4.544613705128157</t>
+          <t>4.548024109543142</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>4.97713731167704</t>
+          <t>4.968394052950249</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.007412545058461</t>
+          <t>1.00771638044802</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>7.008275121520107</t>
+          <t>7.018863192545318</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14.32467743483205</t>
+          <t>14.30659213177179</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2.0246685171009466</t>
+          <t>2.0249631229255742</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5.322568935330892</t>
+          <t>5.32640328305607</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5.401361760961947</t>
+          <t>5.40522224533119</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3.741883589236524</t>
+          <t>3.737871855704123</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>5.919717267418947</t>
+          <t>5.918653708507097</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>16.841726653085438</t>
+          <t>16.84424457928631</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2.7458798428930042</t>
+          <t>2.746403364385035</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3.444268655584417</t>
+          <t>3.44498357515081</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2.542836679912405</t>
+          <t>2.544789606884329</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2.133688271056947</t>
+          <t>2.1355322402961505</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>0.7345069963688591</t>
+          <t>0.7349282260217898</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14.779370914347247</t>
+          <t>14.79052575228991</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>20.592690534500996</t>
+          <t>20.202554779682536</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>4.145017945685868</t>
+          <t>4.137871572923594</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>66.66235213990926</t>
+          <t>75.53734087275534</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2.0367265336869735</t>
+          <t>2.0550087424665264</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4.7041786044181215</t>
+          <t>4.6904200117001515</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>6.2016542407186925</t>
+          <t>6.185120714599598</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4.731574951260397</t>
+          <t>4.712910075774253</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>6.005338958038752</t>
+          <t>5.98917452111926</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>9.921561366611508</t>
+          <t>9.91049401614133</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>6.1963808498610105</t>
+          <t>6.179908529279587</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>4.244322834282525</t>
+          <t>4.231544968281098</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7.248532557356445</t>
+          <t>7.230325301975195</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>10.346652882818672</t>
+          <t>10.335636177509354</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5.769496395535808</t>
+          <t>5.753596095761784</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>0.7052768823542114</t>
+          <t>0.7057354171204595</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>22.94984658231897</t>
+          <t>22.95388476217289</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6.684418640127454</t>
+          <t>6.6857474162912816</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>96.7862678453972</t>
+          <t>96.78167349910503</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>9.855574909396328</t>
+          <t>9.834949930463743</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>43.58059268264996</t>
+          <t>43.48660725790063</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>11.54809473879132</t>
+          <t>12.45242338739863</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>5.79296172981181</t>
+          <t>5.792870089277115</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2.1300586522030267</t>
+          <t>2.1324162546209573</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.7626320669635267</t>
+          <t>1.759583149849845</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.4129770447307437</t>
+          <t>2.4108123467650544</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.3098857553034104</t>
+          <t>1.308197811798181</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>9.740275936547933</t>
+          <t>9.747642269411108</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2.7044788790088</t>
+          <t>2.7052132254043</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>24.827810366997618</t>
+          <t>24.855748049467188</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>5.896282825111442</t>
+          <t>5.869178962246176</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>40.87111442860539</t>
+          <t>40.8951168320198</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>7.255201882181451</t>
+          <t>7.259490745487004</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>22.100106362848848</t>
+          <t>22.1004788736988</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>1.344561252394988</t>
+          <t>1.3455717716039233</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>7.118402266179311</t>
+          <t>7.114400308121961</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2.6452003491139453</t>
+          <t>2.64772765297398</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>5.760951281628627</t>
+          <t>5.764061235966218</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>21.24479906601324</t>
+          <t>21.21411771073802</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>1.1687117473140312</t>
+          <t>1.1704637820302892</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>0.43741491584374104</t>
+          <t>0.43758979377584517</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2.3078804119795677</t>
+          <t>2.3119148846580018</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>5.062104536223866</t>
+          <t>5.071622736239579</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>9.154164301930619</t>
+          <t>9.164076992184583</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2.049054367945791</t>
+          <t>2.0515469862802007</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>3.7694447255371064</t>
+          <t>3.770307462668546</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>0.3756685985989271</t>
+          <t>0.37597752388730604</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>4.606383134619714</t>
+          <t>4.613173510921976</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>0.2938361980686532</t>
+          <t>0.2938871194131131</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2.7777377653366493</t>
+          <t>2.7790200213606404</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>1.5415476633099505</t>
+          <t>1.5429381724920674</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>1.5366765770740098</t>
+          <t>1.5371379841690436</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>0.5765726367923385</t>
+          <t>0.5766293490807008</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>1.8666868020926444</t>
+          <t>1.866942179953085</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>1.8857845986430897</t>
+          <t>1.8869496557045216</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2.595176338952942</t>
+          <t>2.5967256189951096</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>6.051937359014278</t>
+          <t>6.061535597579528</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>3.763693499947238</t>
+          <t>3.7598169538776336</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>3.96984405647109</t>
+          <t>3.977102310729566</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2.3659682268771594</t>
+          <t>2.364702110842875</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>0.8346174301824273</t>
+          <t>0.8345435242855277</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>2.5880738377271513</t>
+          <t>2.5903710691932207</t>
         </is>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>16.61318112226862</t>
+          <t>16.61159760445597</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>9.15053279214219</t>
+          <t>9.167574413979871</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>19.78754117496522</t>
+          <t>19.79604225553276</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>9.59833194162411</t>
+          <t>9.60809745399905</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>22.357290858113505</t>
+          <t>22.372326922838695</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>13.431560537320888</t>
+          <t>13.42000546627794</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>2.9608386981309094</t>
+          <t>2.9633351177829974</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>17.30140178227087</t>
+          <t>17.31134230584965</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>6.386943009185952</t>
+          <t>6.383774019915773</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>4.416625552728682</t>
+          <t>4.40903942137464</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>1.7814210035081697</t>
+          <t>1.7840390227554954</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>2.3554843321073164</t>
+          <t>2.3606454353698547</t>
         </is>
       </c>
     </row>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>0.6947141858971432</t>
+          <t>0.696097880043544</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>5.80468111452241</t>
+          <t>5.811252869765881</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>2.4305834624004348</t>
+          <t>2.4351914080931376</t>
         </is>
       </c>
     </row>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>2.20002032472453</t>
+          <t>2.198737239288866</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>0.28323177374269676</t>
+          <t>0.28384418931991534</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>0.3625160056077975</t>
+          <t>0.36272899202234754</t>
         </is>
       </c>
     </row>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>0.4073344279239269</t>
+          <t>0.40680695568551983</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>2.0581513375229585</t>
+          <t>2.0631122721488673</t>
         </is>
       </c>
     </row>
@@ -4939,7 +4939,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>1.3747447007115206</t>
+          <t>1.3778231213128702</t>
         </is>
       </c>
     </row>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>1.1493518974489787</t>
+          <t>1.1513359738702909</t>
         </is>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>0.35989552172144706</t>
+          <t>0.35994806169069243</t>
         </is>
       </c>
     </row>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>0.8559175129745157</t>
+          <t>0.8570983944895296</t>
         </is>
       </c>
     </row>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>12.497970656994898</t>
+          <t>12.489790205676222</t>
         </is>
       </c>
     </row>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>82.28086548853786</t>
+          <t>82.33539619162269</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>17.82812392743921</t>
+          <t>17.8598189530847</t>
         </is>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>17.336941334911018</t>
+          <t>17.31511670490435</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>95.3296974837797</t>
+          <t>95.77899130394034</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>15.987841789556805</t>
+          <t>15.986454877423068</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Toppo Banner added - not summoning
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -5330,12 +5330,12 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>16.111457504315194</t>
+          <t>6.68491054074687</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add AGL Dabura & Babidi
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D243"/>
+  <dimension ref="A1:D244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.126409615703768</t>
+          <t>6.139187248922411</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6.299025608177714</t>
+          <t>6.299252947052693</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.551940117044956</t>
+          <t>2.550440564538791</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.5567069214352767</t>
+          <t>1.5638155202842765</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.4400677834812505</t>
+          <t>4.45878644481067</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.3089630611547722</t>
+          <t>2.316705278844881</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5.438720539843782</t>
+          <t>5.458490992683864</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6.431256229306559</t>
+          <t>6.448982713151821</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5.649024600226481</t>
+          <t>5.659956984522379</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.059622672872867</t>
+          <t>2.0657664196040004</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>11.900908065753761</t>
+          <t>11.91705747038271</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.7582921951485071</t>
+          <t>0.7631217896196449</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6.8046969361695275</t>
+          <t>6.828444916708278</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10.057325323279041</t>
+          <t>10.074871387836708</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5.30835842789118</t>
+          <t>5.324663511065344</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13.66104025001445</t>
+          <t>13.625070099797988</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>6.924395186439783</t>
+          <t>6.940239084363435</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7.092286234370638</t>
+          <t>7.092492268063044</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12.89522762875426</t>
+          <t>12.94681927865114</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6.302908904314965</t>
+          <t>6.307336815643707</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.8670281694194908</t>
+          <t>0.872476553881592</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7.538160886955179</t>
+          <t>7.559263188369169</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.1673975032969413</t>
+          <t>2.181871335400589</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>5.086198149983105</t>
+          <t>5.104466944348533</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3.758451177709153</t>
+          <t>3.7754910853667396</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>18.29012463323369</t>
+          <t>18.36624211695437</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12.842934517501716</t>
+          <t>12.847084081328298</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12.785995248542182</t>
+          <t>12.802063428896101</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4.64113372913355</t>
+          <t>4.644025760502991</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>4.90139506024834</t>
+          <t>4.918895131342344</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.9900661890465906</t>
+          <t>0.9907969195193295</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>6.9371523073015595</t>
+          <t>6.926561291691385</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>15.42020587100708</t>
+          <t>15.44001656524471</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.9813752129402813</t>
+          <t>1.9869563239945651</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5.385520699568108</t>
+          <t>5.402236243701537</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5.964555768226057</t>
+          <t>5.970765865259975</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3.681720034147137</t>
+          <t>3.690460081922671</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>5.695692827540766</t>
+          <t>5.707702608445341</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>16.54881142933445</t>
+          <t>16.53938918826345</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2.326244459100528</t>
+          <t>2.319147478378109</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2.1147665768293678</t>
+          <t>2.1156345751100005</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4.065172888453759</t>
+          <t>4.066872442469233</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>20.674298041111967</t>
+          <t>20.693688200157062</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.4318649802935806</t>
+          <t>1.4390032128066501</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14.975056973014276</t>
+          <t>14.921779324807789</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2.172683459669571</t>
+          <t>2.165978224523357</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4.504903565657519</t>
+          <t>4.526041727350825</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>5.9705835036177435</t>
+          <t>5.998706346952921</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4.4902994596248655</t>
+          <t>4.511356410298207</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>5.7807307691137515</t>
+          <t>5.811342098454194</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>9.583253009680035</t>
+          <t>9.619963275700336</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>5.957342976306959</t>
+          <t>5.988242591301891</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>4.06474430829893</t>
+          <t>4.083712514845842</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>6.951665907740321</t>
+          <t>6.986453669886759</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>10.016148483738107</t>
+          <t>10.054401063901981</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5.559923807801083</t>
+          <t>5.5880804407076194</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>0.698555100013008</t>
+          <t>0.7003229135392982</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>22.41543408372273</t>
+          <t>22.4665348785196</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6.6277405106475955</t>
+          <t>6.64447598658541</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.9399113517551285</t>
+          <t>1.9421795582701122</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>42.7413615362914</t>
+          <t>42.61502106224913</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>11.94913843781582</t>
+          <t>11.92892515186385</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>5.626087734619789</t>
+          <t>5.631115153920776</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2.1076350430196484</t>
+          <t>2.1118098995514942</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>0.501551590677523</t>
+          <t>0.5036889623490559</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.419123308367877</t>
+          <t>2.4296087760503817</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.2802175397184747</t>
+          <t>1.284580260784546</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>9.727256792443308</t>
+          <t>9.734242536085787</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2.662755031353509</t>
+          <t>2.6739551634150907</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>24.407113438424492</t>
+          <t>24.472467565623347</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>7.127010725970761</t>
+          <t>7.162944270766605</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>40.19242108016971</t>
+          <t>40.15589117356571</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>6.85533490579601</t>
+          <t>6.857380409802685</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>22.34176106137726</t>
+          <t>22.336005402446638</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>3.945229612868607</t>
+          <t>3.952111760008849</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>5.73562871380233</t>
+          <t>5.76940050110566</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>20.53854485614647</t>
+          <t>20.49242591562365</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>1.1670251293044718</t>
+          <t>1.1699285959969288</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>0.42575198181422813</t>
+          <t>0.4267223156846239</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2.28746993334709</t>
+          <t>2.2937221340903804</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>5.09197268785061</t>
+          <t>5.106976026784182</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>9.254617263976998</t>
+          <t>9.274883747889975</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>1.95070100058037</t>
+          <t>1.9567379787105104</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>1.4867817415782805</t>
+          <t>1.4897124396696813</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>0.36271995833314513</t>
+          <t>0.36408159941510554</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>4.577154571608736</t>
+          <t>4.597811242606415</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>0.2888948090435106</t>
+          <t>0.2895863641272225</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2.769701129387432</t>
+          <t>2.776964792931107</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>1.5335149713641565</t>
+          <t>1.5381899971039779</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>1.8561857265346617</t>
+          <t>1.8543667734045215</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>1.8249597928856305</t>
+          <t>1.8315466354785563</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2.5705162587520896</t>
+          <t>2.5828724620759247</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>4.943733007236769</t>
+          <t>4.970218964301331</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>3.730517488403736</t>
+          <t>3.74166576990495</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>2.5830098804224004</t>
+          <t>2.5839983187972813</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2.35110205339861</t>
+          <t>2.3593819591171354</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>2.578507305376714</t>
+          <t>2.5821160962015046</t>
         </is>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>15.91952811876748</t>
+          <t>15.977242179068417</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>9.133940736434642</t>
+          <t>9.14010952826337</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>11.774826206985512</t>
+          <t>11.810951666129451</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>8.537087790352942</t>
+          <t>8.518475146912962</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>19.266593360210194</t>
+          <t>19.258436497742636</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>14.38637762556562</t>
+          <t>14.4278972227444</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>2.8018570270631704</t>
+          <t>2.8034719683155913</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>18.12971536886753</t>
+          <t>18.1841111734711</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>6.512118813350172</t>
+          <t>6.526503692515929</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>5.313512560091958</t>
+          <t>5.3192563247689115</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>1.168902502418523</t>
+          <t>1.173478565158951</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>2.373360523249684</t>
+          <t>2.385417302576425</t>
         </is>
       </c>
     </row>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>0.6912866627073113</t>
+          <t>0.6940123891396761</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>2.716646426484445</t>
+          <t>2.7177053905664437</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>2.4690431560469346</t>
+          <t>2.480946525749612</t>
         </is>
       </c>
     </row>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>2.8782977113309807</t>
+          <t>2.8739256230049524</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>0.28707406833839955</t>
+          <t>0.2881046890303508</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>0.36330149736105855</t>
+          <t>0.3639387552098146</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>0.6482138192907776</t>
+          <t>0.6509053371819391</t>
         </is>
       </c>
     </row>
@@ -4939,7 +4939,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>1.3621073559153398</t>
+          <t>1.3687424350434405</t>
         </is>
       </c>
     </row>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>1.538443165003261</t>
+          <t>1.5464764274893295</t>
         </is>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>0.3488490274794336</t>
+          <t>0.34913852280593916</t>
         </is>
       </c>
     </row>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>0.8443234103511326</t>
+          <t>0.8472346096249985</t>
         </is>
       </c>
     </row>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>12.108026872889452</t>
+          <t>12.153908579282296</t>
         </is>
       </c>
     </row>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>83.51968800609593</t>
+          <t>83.61409325510712</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>18.06876637487641</t>
+          <t>18.17057213535799</t>
         </is>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>16.535620643718804</t>
+          <t>16.58286775663775</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>95.48386506375664</t>
+          <t>95.47701527595419</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>6.724168294220314</t>
+          <t>6.715618877039381</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>1.1225672156071296</t>
+          <t>1.1289840818987298</t>
         </is>
       </c>
     </row>
@@ -5445,7 +5445,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>1.1616092181773223</t>
+          <t>1.1671052274681861</t>
         </is>
       </c>
     </row>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>3.4748629908767406</t>
+          <t>3.493344367139362</t>
         </is>
       </c>
     </row>
@@ -5511,7 +5511,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>63.72728811026222</t>
+          <t>63.842521077989495</t>
         </is>
       </c>
     </row>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>4.105335093526613</t>
+          <t>4.0977566023258625</t>
         </is>
       </c>
     </row>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>22.85000487164185</t>
+          <t>22.84587198105828</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>24.16530135561232</t>
+          <t>24.25976922473372</t>
         </is>
       </c>
     </row>
@@ -5621,7 +5621,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>0.9523597765956043</t>
+          <t>0.9583773125760349</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>3.610958487977693</t>
+          <t>3.612378878172543</t>
         </is>
       </c>
     </row>
@@ -5731,7 +5731,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>3.463730656213336</t>
+          <t>3.478336067007227</t>
         </is>
       </c>
     </row>
@@ -5753,7 +5753,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>14.78089073715648</t>
+          <t>14.87333252412737</t>
         </is>
       </c>
     </row>
@@ -5775,7 +5775,29 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>8.789498404718787</t>
+          <t>8.78950483384065</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="inlineStr">
+        <is>
+          <t>243</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>F2P_STR_Devilman</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>0.2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add LR Teq Broly
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.1761997561382</t>
+          <t>6.27196838560652</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>6.261533567078409</t>
+          <t>6.136354835926184</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>25.29252225921852</t>
+          <t>23.509476198650532</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.5498837160909842</t>
+          <t>1.584696893011312</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.639710239535049</t>
+          <t>4.688808836676181</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.3014882487834023</t>
+          <t>2.2905643788719434</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5.662844386804879</t>
+          <t>5.734912096518487</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.6682649272004906</t>
+          <t>1.6753556110092993</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6.450576435437661</t>
+          <t>6.541911308728249</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5.646585011273011</t>
+          <t>5.886762516609979</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.0459997236190732</t>
+          <t>2.146053574743428</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>11.7772644682311</t>
+          <t>12.98047152253207</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.7386760762670153</t>
+          <t>0.7234971861536101</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6.78819350685281</t>
+          <t>6.866365819764088</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10.06924993843175</t>
+          <t>10.245469935640859</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6.248983935516343</t>
+          <t>6.29160872534187</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>10.852321928038528</t>
+          <t>11.018468912105938</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>7.179150673394268</t>
+          <t>7.152297099787099</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7.092374830228623</t>
+          <t>7.210113871109218</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12.71228262309772</t>
+          <t>12.09374316632322</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6.2691140747968115</t>
+          <t>6.332326452833407</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1.238472485079381</t>
+          <t>1.2635684915844116</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>7.59295532382119</t>
+          <t>7.781611118422028</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.1580349465042445</t>
+          <t>2.1513597362620587</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4.989669282024708</t>
+          <t>5.171761187494893</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3.7538260956315868</t>
+          <t>3.9636913462593437</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>18.26035709095147</t>
+          <t>18.19400847987445</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>12.801121936850805</t>
+          <t>12.884274223427347</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12.844309569735099</t>
+          <t>13.200514128466672</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4.6399962271022375</t>
+          <t>4.66039607279675</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2.095053477143238</t>
+          <t>2.1230975901873697</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>0.9889577913475308</t>
+          <t>1.0040445720405273</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>6.85646429257421</t>
+          <t>6.83738540339381</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>15.26035289368773</t>
+          <t>15.28445289821045</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2.704734241624033</t>
+          <t>2.7130868873672878</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.11056472217928</t>
+          <t>1.0755411064328406</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5.992725044456816</t>
+          <t>6.00906215503591</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>4.543503104997161</t>
+          <t>4.62968795413693</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>5.562074645318099</t>
+          <t>5.542216299404848</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>16.470868659171213</t>
+          <t>16.74742378176302</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2.3954207443646083</t>
+          <t>2.3076328123176046</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2.08230582741443</t>
+          <t>2.106622385789791</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4.043039430907342</t>
+          <t>4.0286901508141995</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>20.662354919418917</t>
+          <t>20.442903340017985</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2.46839831241463</t>
+          <t>2.5501419271780286</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14.53443631087714</t>
+          <t>13.6804682030198</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2.1888533436486597</t>
+          <t>2.4220035393696264</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4.439294500472511</t>
+          <t>4.68156252986687</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>5.906425715555656</t>
+          <t>6.233351105632052</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4.428806794912898</t>
+          <t>4.7339543508277915</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>5.708933336395822</t>
+          <t>6.024746763569873</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>9.554413401793552</t>
+          <t>10.07837979450683</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>5.899945382444045</t>
+          <t>6.224482556918865</t>
         </is>
       </c>
     </row>
@@ -2079,7 +2079,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>3.9986486214845383</t>
+          <t>4.2155511352192905</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>6.880349416533448</t>
+          <t>7.263918479230486</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2123,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>10.004390013316739</t>
+          <t>10.545856472532163</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5.468555844262781</t>
+          <t>5.7748675265611285</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>0.6931906373157</t>
+          <t>0.7016824516676934</t>
         </is>
       </c>
     </row>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>16.088607900086814</t>
+          <t>16.295305005463423</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6.590764467129763</t>
+          <t>6.708318540976928</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.9086324655969236</t>
+          <t>1.944378707467905</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>42.21861929290034</t>
+          <t>44.86763513446393</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>11.69235026401818</t>
+          <t>12.27101897339271</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>5.567557255538703</t>
+          <t>5.615344696420776</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2.8500657330338663</t>
+          <t>2.8789061091526285</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>0.5001274064732879</t>
+          <t>0.5238995814089504</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2.432346245031103</t>
+          <t>2.548417848004698</t>
         </is>
       </c>
     </row>
@@ -2409,7 +2409,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>1.263149006081679</t>
+          <t>1.303295730612597</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>4.954103614129071</t>
+          <t>4.972152807475088</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>3.6944051059227117</t>
+          <t>3.817697154822909</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>23.910040862609627</t>
+          <t>24.136761557510074</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>7.159998116193362</t>
+          <t>7.723549321351261</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>39.74682088549973</t>
+          <t>40.04055738608627</t>
         </is>
       </c>
     </row>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>6.818563855402165</t>
+          <t>6.923468572478091</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>22.578436279623165</t>
+          <t>22.95258299768636</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>3.901208753740585</t>
+          <t>3.948770294332424</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>5.673410506115455</t>
+          <t>5.655213602373385</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>20.5905538170784</t>
+          <t>21.08525021080629</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>1.2246648890901497</t>
+          <t>1.211713364778042</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>0.42496004143048177</t>
+          <t>0.4316869338532308</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2.2707863268986586</t>
+          <t>2.2165629762473387</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>5.0802461053922565</t>
+          <t>5.116751283827598</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>9.29488343825488</t>
+          <t>9.13877082498881</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2.0399371109842495</t>
+          <t>2.050253205115359</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2.7436300837727607</t>
+          <t>2.7813885309813706</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>0.35574497887034207</t>
+          <t>0.3606149969140208</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>4.574557058192846</t>
+          <t>4.5615814147754</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>0.28312762457201096</t>
+          <t>0.2858987981237951</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2.803245667292572</t>
+          <t>2.8559498374146486</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>1.8839221834923452</t>
+          <t>1.8763862501753152</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>1.8544828357978655</t>
+          <t>1.8762912529329743</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2.5444742245384457</t>
+          <t>2.5397560042832317</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>4.890499804244268</t>
+          <t>4.91254881570476</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>3.6519374677714573</t>
+          <t>3.758994919541685</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>2.589455714009901</t>
+          <t>2.585438973340029</t>
         </is>
       </c>
     </row>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>2.533407238995632</t>
+          <t>2.5719140803979985</t>
         </is>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>18.46453656667308</t>
+          <t>19.73902752452125</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>8.979214768157831</t>
+          <t>9.085272102455669</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>4.769281485517219</t>
+          <t>4.823494542553675</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>8.14265052912603</t>
+          <t>8.401665664951665</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>19.331218435085987</t>
+          <t>19.35952627242804</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>14.23323565739505</t>
+          <t>14.40774155666486</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>17.81147002240777</t>
+          <t>18.03923170433676</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>3.2038219189706223</t>
+          <t>3.283483355697279</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>5.375815492396679</t>
+          <t>5.673571529756462</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>1.22689666526421</t>
+          <t>1.2321072374476332</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>2.385440245042159</t>
+          <t>2.3721855991535024</t>
         </is>
       </c>
     </row>
@@ -4543,7 +4543,7 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>2.6844575702526257</t>
+          <t>2.724837940032252</t>
         </is>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>2.462364049782618</t>
+          <t>2.465922202199149</t>
         </is>
       </c>
     </row>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>2.893057428532037</t>
+          <t>2.9631810104565535</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>0.36507196013697446</t>
+          <t>0.3684931111189188</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>0.4778751028623507</t>
+          <t>0.4772027855296699</t>
         </is>
       </c>
     </row>
@@ -4939,7 +4939,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>1.3487512833959112</t>
+          <t>1.3493201348164785</t>
         </is>
       </c>
     </row>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>1.547474822455846</t>
+          <t>1.5453943695395924</t>
         </is>
       </c>
     </row>
@@ -4983,7 +4983,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>0.3510948308949001</t>
+          <t>0.36384741130444404</t>
         </is>
       </c>
     </row>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>0.8773572779953638</t>
+          <t>0.8825986555297346</t>
         </is>
       </c>
     </row>
@@ -5093,7 +5093,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>12.05255854912553</t>
+          <t>12.674799649278976</t>
         </is>
       </c>
     </row>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>84.5756457248159</t>
+          <t>83.75348144104282</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5203,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>17.79793497765765</t>
+          <t>17.75948706024397</t>
         </is>
       </c>
     </row>
@@ -5225,7 +5225,7 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>16.120820923335085</t>
+          <t>17.27012310781259</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>95.49524167861007</t>
+          <t>96.04541329955238</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>6.83298784665584</t>
+          <t>6.80218405877913</t>
         </is>
       </c>
     </row>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>1.1149665067994852</t>
+          <t>1.1094086786473205</t>
         </is>
       </c>
     </row>
@@ -5445,7 +5445,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>1.1721546610747886</t>
+          <t>1.2057971265882266</t>
         </is>
       </c>
     </row>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>3.483334870108532</t>
+          <t>3.630183782833331</t>
         </is>
       </c>
     </row>
@@ -5511,7 +5511,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>63.84580545753785</t>
+          <t>64.60298952384126</t>
         </is>
       </c>
     </row>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>4.082706881167346</t>
+          <t>4.080301201502997</t>
         </is>
       </c>
     </row>
@@ -5555,7 +5555,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>22.72852118755638</t>
+          <t>23.8292651689578</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>23.959037259042</t>
+          <t>25.20227357153311</t>
         </is>
       </c>
     </row>
@@ -5621,7 +5621,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>0.948280582427203</t>
+          <t>0.9435133914578074</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>3.6608538314544132</t>
+          <t>3.7856456702044596</t>
         </is>
       </c>
     </row>
@@ -5731,7 +5731,7 @@
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>3.367530525655629</t>
+          <t>3.44777946826958</t>
         </is>
       </c>
     </row>
@@ -5753,7 +5753,7 @@
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>14.12487146318295</t>
+          <t>14.85533565172542</t>
         </is>
       </c>
     </row>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>8.808238971407485</t>
+          <t>8.739159796001914</t>
         </is>
       </c>
     </row>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>3.1330972881954677</t>
+          <t>3.186022020299646</t>
         </is>
       </c>
     </row>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>4.9481259939009306</t>
+          <t>4.847212550506001</t>
         </is>
       </c>
     </row>
@@ -5863,7 +5863,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>73.58845485885423</t>
+          <t>75.77554007213239</t>
         </is>
       </c>
     </row>
@@ -5885,7 +5885,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>9.290401318079923</t>
+          <t>9.310338775294527</t>
         </is>
       </c>
     </row>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>5.074478867426137</t>
+          <t>5.393747368852728</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add STR DF Broly
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -1084,12 +1084,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.264946657132045</t>
+          <t>2.3369175545322847</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Nail to be less busted
</commit_message>
<xml_diff>
--- a/SummonRating.xlsx
+++ b/SummonRating.xlsx
@@ -1106,12 +1106,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3.600480817052625</t>
+          <t>5.233906821501709</t>
         </is>
       </c>
     </row>
@@ -2646,12 +2646,12 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>20.206535434077573</t>
+          <t>11.497509829856869</t>
         </is>
       </c>
     </row>
@@ -6166,12 +6166,12 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>58.34455620081922</t>
+          <t>6.273954516817895</t>
         </is>
       </c>
     </row>

</xml_diff>